<commit_message>
removendo cookie e desativando vendedor
</commit_message>
<xml_diff>
--- a/Setor Cancelamento.xlsx
+++ b/Setor Cancelamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DirectUser\Documents\Scripts\criar_usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4888CD48-A2F5-46F8-8298-F290B8218A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD8F7C1-B721-42FE-BDF3-53192D86BD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Geral</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>HubSoft TI</t>
@@ -432,9 +429,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
@@ -482,10 +479,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
@@ -499,32 +496,6 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>